<commit_message>
kemiskinan done modelling | pengangguran scraping
</commit_message>
<xml_diff>
--- a/compile/compiled_data_normalized_ver2.xlsx
+++ b/compile/compiled_data_normalized_ver2.xlsx
@@ -61,7 +61,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -122,14 +122,14 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -448,16 +448,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="15.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="15.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="8" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="8" width="9.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -492,7 +492,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3">
         <v>2010</v>
       </c>
@@ -524,7 +524,7 @@
         <v>21.29765844077476</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3">
         <v>2011</v>
       </c>
@@ -556,7 +556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3">
         <v>2012</v>
       </c>
@@ -588,7 +588,7 @@
         <v>21.29765844077476</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3">
         <v>2013</v>
       </c>
@@ -620,7 +620,7 @@
         <v>21.29765844077476</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3">
         <v>2014</v>
       </c>
@@ -652,7 +652,7 @@
         <v>21.29765844077476</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3">
         <v>2015</v>
       </c>
@@ -684,7 +684,7 @@
         <v>21.29765844077476</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3">
         <v>2016</v>
       </c>
@@ -716,7 +716,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3">
         <v>2017</v>
       </c>
@@ -748,7 +748,7 @@
         <v>24.27184466019418</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3">
         <v>2018</v>
       </c>
@@ -780,7 +780,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3">
         <v>2019</v>
       </c>
@@ -812,7 +812,7 @@
         <v>20.83333333333334</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3">
         <v>2020</v>
       </c>
@@ -844,7 +844,7 @@
         <v>21.59827213822894</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3">
         <v>2021</v>
       </c>
@@ -876,7 +876,7 @@
         <v>22.4618149146451</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3">
         <v>2022</v>
       </c>
@@ -908,7 +908,7 @@
         <v>23.14814814814815</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3">
         <v>2023</v>
       </c>
@@ -940,7 +940,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="3">
         <v>2024</v>
       </c>

</xml_diff>